<commit_message>
Refactor project structure and enhance functionality
- Updated .gitignore to include new directories and files for better management.
- Reformatted chat_ids.json for improved readability.
- Removed deprecated chat_manager.py file to streamline the codebase.
- Updated bot_token in config.py for security.
- Enhanced events.json with new event entries and improved structure.
- Refactored main.py to utilize async features and improve application startup.
- Updated message_handler.py to fix import paths and improve event handling.
- Removed package-lock.json and package.json files to clean up unused dependencies.
- Updated user_data.json and other JSON files for better data management.
- Improved access control and mediator functionalities in utils.
- Enhanced web application with new routes and improved CORS settings.
- Updated React components for better performance and user experience.
- Added new styles and improved existing ones for better UI consistency.
</commit_message>
<xml_diff>
--- a/output/inventory.xlsx
+++ b/output/inventory.xlsx
@@ -457,14 +457,14 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Дата: 2024-12-17</t>
+          <t>Дата: 2024-12-21</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Время: 07:49:34</t>
+          <t>Время: 06:47:38</t>
         </is>
       </c>
     </row>

</xml_diff>